<commit_message>
add,remove permissions in group, comment the code to add user to the group
</commit_message>
<xml_diff>
--- a/ProjectSchema/rtbSchema.xlsx
+++ b/ProjectSchema/rtbSchema.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Atebal Kant Singh\DjangoWorkspace\canteen\ProjectSchema\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1ED7BD7-4E36-4CBD-99F0-5271D7F3F1A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35B494FD-FCC1-43E2-B466-293A694FDD96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{425E41E4-B678-41BD-80BC-54B9EBB65333}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="89">
   <si>
     <t>UsrName</t>
   </si>
@@ -368,19 +368,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4695,223 +4694,124 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-    </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="5"/>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="5"/>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="5"/>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="5"/>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="5"/>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="5"/>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="5"/>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="5"/>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B14" s="8"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
+      <c r="B14" s="6"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="5"/>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="I15" s="3"/>
+      <c r="I15" s="2"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="5"/>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="5"/>
-      <c r="B17" s="8" t="s">
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B17" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="5"/>
-      <c r="B18" s="8" t="s">
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B18" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="5"/>
-      <c r="B19" s="8" t="s">
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B19" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="5"/>
-      <c r="B20" s="8" t="s">
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B20" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="5"/>
-      <c r="B21" s="8" t="s">
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B21" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="5"/>
-      <c r="B22" s="8" t="s">
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B22" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4928,7 +4828,7 @@
   <dimension ref="A5:C36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5047,6 +4947,9 @@
       <c r="A19" t="s">
         <v>71</v>
       </c>
+      <c r="C19" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">

</xml_diff>